<commit_message>
Fix tests, bootstrap data
</commit_message>
<xml_diff>
--- a/scripts/bootstrap/measurement_data/synthetic_gut.xlsx
+++ b/scripts/bootstrap/measurement_data/synthetic_gut.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Growth data per community" sheetId="1" state="visible" r:id="rId3"/>
@@ -425,7 +425,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="32">
   <si>
     <t xml:space="preserve">Biological Replicate</t>
   </si>
@@ -460,9 +460,6 @@
     <t xml:space="preserve">biorep6</t>
   </si>
   <si>
-    <t xml:space="preserve">biorepBlank</t>
-  </si>
-  <si>
     <t xml:space="preserve">Roseburia intestinalis rRNA reads</t>
   </si>
   <si>
@@ -481,16 +478,16 @@
     <t xml:space="preserve">Prevotella copri DSM 18205 rRNA reads STD</t>
   </si>
   <si>
+    <t xml:space="preserve">Bacteroides thetaiotaomicron rRNA reads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteroides thetaiotaomicron rRNA reads STD</t>
+  </si>
+  <si>
     <t xml:space="preserve">Collinsella aerofaciens rRNA reads</t>
   </si>
   <si>
     <t xml:space="preserve">Collinsella aerofaciens rRNA reads STD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bacteroides thetaiotaomicron rRNA reads</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bacteroides thetaiotaomicron rRNA reads STD</t>
   </si>
   <si>
     <t xml:space="preserve">pyruvate</t>
@@ -931,14 +928,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" activeCellId="1" sqref="D38:M43 C2"/>
+      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1467,90 +1464,12 @@
         <v>331865000</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="D38" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="D39" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="D40" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="D41" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="D42" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="D43" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1568,14 +1487,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M26" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="J23" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
-      <selection pane="bottomRight" activeCell="D38" activeCellId="0" sqref="D38:M43"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="J38" activeCellId="0" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1606,34 +1525,34 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3112,82 +3031,12 @@
         <v>8444221.28538469</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="1" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="1" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="1" t="n">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3205,14 +3054,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="I2" activeCellId="1" sqref="D38:M43 I2"/>
+      <selection pane="bottomRight" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3243,37 +3092,37 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4852,72 +4701,12 @@
         <v>1887.18</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="1" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="1" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="1" t="n">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="1" t="n">
-        <v>67</v>
-      </c>
-    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>